<commit_message>
Added Code changes for Creative Delivery Hierarchy Careative ID
</commit_message>
<xml_diff>
--- a/Datorama_Creative_Hierarchcial.xlsx
+++ b/Datorama_Creative_Hierarchcial.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CreativeDelivery_CampaignTarget" sheetId="1" r:id="rId1"/>
+    <sheet name="CreativeDelivery_CreativeID" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
   <si>
     <t>sourceColumn</t>
   </si>
@@ -78,6 +79,12 @@
   </si>
   <si>
     <t>SUBSTRING</t>
+  </si>
+  <si>
+    <t>creative_id</t>
+  </si>
+  <si>
+    <t>Creative ID</t>
   </si>
 </sst>
 </file>
@@ -431,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,4 +539,109 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Creative Level Campaign and Advertiser Hierarchy
</commit_message>
<xml_diff>
--- a/Datorama_Creative_Hierarchcial.xlsx
+++ b/Datorama_Creative_Hierarchcial.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="CreativeDelivery_CampaignTarget" sheetId="1" r:id="rId1"/>
     <sheet name="CreativeDelivery_CreativeID" sheetId="2" r:id="rId2"/>
+    <sheet name="CreativeDelivery_AdvertiserID" sheetId="3" r:id="rId3"/>
+    <sheet name="CreativeDelivery_CampaignID" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="23">
   <si>
     <t>sourceColumn</t>
   </si>
@@ -85,6 +87,15 @@
   </si>
   <si>
     <t>Creative ID</t>
+  </si>
+  <si>
+    <t>advertiser_id</t>
+  </si>
+  <si>
+    <t>Advertiser ID</t>
+  </si>
+  <si>
+    <t>Campaign ID</t>
   </si>
 </sst>
 </file>
@@ -545,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,5 +654,220 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added the display level changes to the framework
</commit_message>
<xml_diff>
--- a/Datorama_Creative_Hierarchcial.xlsx
+++ b/Datorama_Creative_Hierarchcial.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\DatoramaMain\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\stash\datorama-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9516" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="CreativeDelivery_CampaignTarget" sheetId="1" r:id="rId1"/>
@@ -66,15 +66,6 @@
     <t>total_impressions</t>
   </si>
   <si>
-    <t>Impressions</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
-    <t>Clicks</t>
-  </si>
-  <si>
     <t>total_cost</t>
   </si>
   <si>
@@ -105,16 +96,25 @@
     <t>total_click_based_conversion</t>
   </si>
   <si>
-    <t>Click Based Conversions</t>
-  </si>
-  <si>
     <t>total_view_based_conversion</t>
   </si>
   <si>
-    <t>View Based Conversions</t>
-  </si>
-  <si>
     <t>Campaign_ID</t>
+  </si>
+  <si>
+    <t>Impressions (IOne)</t>
+  </si>
+  <si>
+    <t>Media Cost (IOne)</t>
+  </si>
+  <si>
+    <t>Clicks (IOne)</t>
+  </si>
+  <si>
+    <t>Click Based Conversions (IOne)</t>
+  </si>
+  <si>
+    <t>View Based Conversions (IOne)</t>
   </si>
 </sst>
 </file>
@@ -469,19 +469,19 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -498,7 +498,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -515,12 +515,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
@@ -529,32 +529,32 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -563,7 +563,7 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -576,17 +576,17 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E5"/>
+      <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -603,12 +603,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -620,12 +620,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
@@ -634,32 +634,32 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -668,7 +668,7 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -682,19 +682,19 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E5"/>
+      <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -711,12 +711,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -728,12 +728,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
@@ -742,32 +742,32 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -776,7 +776,7 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -789,19 +789,19 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -818,12 +818,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -835,12 +835,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
@@ -849,32 +849,32 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -883,7 +883,7 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -895,20 +895,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -925,7 +925,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -942,35 +942,35 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
@@ -986,19 +986,19 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1015,12 +1015,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -1032,35 +1032,35 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
@@ -1076,19 +1076,19 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1105,12 +1105,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -1122,35 +1122,35 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
@@ -1165,20 +1165,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1195,12 +1195,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -1212,35 +1212,35 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Added Creative Level test for placement ID level
</commit_message>
<xml_diff>
--- a/Datorama_Creative_Hierarchcial.xlsx
+++ b/Datorama_Creative_Hierarchcial.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="CreativeDelivery_CampaignTarget" sheetId="1" r:id="rId1"/>
     <sheet name="CreativeDelivery_CreativeID" sheetId="2" r:id="rId2"/>
     <sheet name="CreativeDelivery_AdvertiserID" sheetId="3" r:id="rId3"/>
-    <sheet name="CreativeDelivery_CampaignID" sheetId="4" r:id="rId4"/>
-    <sheet name="CreativeConv_CampaignTarget" sheetId="5" r:id="rId5"/>
-    <sheet name="CreativeConv_Creative" sheetId="6" r:id="rId6"/>
-    <sheet name="CreativeConv_Campaign" sheetId="7" r:id="rId7"/>
-    <sheet name="CreativeConv_Advertiser" sheetId="8" r:id="rId8"/>
+    <sheet name="CreativeDelivery_PlacementID" sheetId="9" r:id="rId4"/>
+    <sheet name="CreativeDelivery_CampaignID" sheetId="4" r:id="rId5"/>
+    <sheet name="CreativeConv_CampaignTarget" sheetId="5" r:id="rId6"/>
+    <sheet name="CreativeConv_Creative" sheetId="6" r:id="rId7"/>
+    <sheet name="CreativeConv_Campaign" sheetId="7" r:id="rId8"/>
+    <sheet name="CreativeConv_Advertiser" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="30">
   <si>
     <t>sourceColumn</t>
   </si>
@@ -115,6 +116,12 @@
   </si>
   <si>
     <t>View Based Conversions (IOne)</t>
+  </si>
+  <si>
+    <t>Adserver Placement ID</t>
+  </si>
+  <si>
+    <t>Adserver_Placement_ID</t>
   </si>
 </sst>
 </file>
@@ -682,7 +689,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B5"/>
+      <selection sqref="A1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,6 +792,113 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -891,7 +1005,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -931,96 +1045,6 @@
       </c>
       <c r="B2" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -1107,10 +1131,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -1165,7 +1189,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
@@ -1197,6 +1221,96 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>17</v>
       </c>
       <c r="B2" t="s">

</xml_diff>